<commit_message>
changed how the information is saved. Integrated technical and fundamental scores into the total final score. Changed how the trader works. Allowing for half trades and strong trades. Updated the excel methods to save the new trading data
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="10215"/>
   </bookViews>
   <sheets>
     <sheet name="WorkSheet 1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>totalScore</t>
+    <t>ScoreFinal</t>
+  </si>
+  <si>
+    <t>totalSentiment</t>
   </si>
   <si>
     <t>posWordPercentage</t>
@@ -66,6 +69,12 @@
   </si>
   <si>
     <t>Method</t>
+  </si>
+  <si>
+    <t>RSI</t>
+  </si>
+  <si>
+    <t>PEG</t>
   </si>
   <si>
     <t>Bag</t>
@@ -387,28 +396,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,49 +460,120 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42614.524328703701</v>
+        <v>42627.87427083333</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E2">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F2">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="G2">
-        <v>97504</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>37284</v>
+        <v>5231</v>
       </c>
       <c r="I2">
-        <v>3436</v>
+        <v>7031</v>
       </c>
       <c r="J2">
-        <v>473</v>
+        <v>743</v>
       </c>
       <c r="K2">
-        <v>366</v>
+        <v>122</v>
       </c>
       <c r="L2">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="M2">
-        <v>13</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42627.877280092594</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>3067</v>
+      </c>
+      <c r="I3">
+        <v>5351</v>
+      </c>
+      <c r="J3">
+        <v>545</v>
+      </c>
+      <c r="K3">
+        <v>81</v>
+      </c>
+      <c r="L3">
+        <v>46</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A lot of changes. Added more information to sentiment excel sheet to include an up down category. The trader now trades in Long and Hold trades. This is still in the testing period
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -95,10 +95,19 @@
     <t>Bollinger</t>
   </si>
   <si>
-    <t>Neutral</t>
+    <t>PriceChange</t>
+  </si>
+  <si>
+    <t>UpDown</t>
+  </si>
+  <si>
+    <t>Buy</t>
   </si>
   <si>
     <t>Bag</t>
+  </si>
+  <si>
+    <t>Down</t>
   </si>
 </sst>
 </file>
@@ -418,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,7 +435,7 @@
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -439,7 +448,7 @@
     <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,75 +518,158 @@
       <c r="W1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42629.656793981485</v>
+        <v>42633.878900462965</v>
       </c>
       <c r="B2">
-        <v>-5</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="E2">
-        <v>25156</v>
+        <v>10620</v>
       </c>
       <c r="F2">
-        <v>2311</v>
+        <v>1266</v>
       </c>
       <c r="G2">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="H2">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I2">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>6892</v>
+      </c>
+      <c r="L2">
+        <v>139</v>
+      </c>
+      <c r="M2">
+        <v>81</v>
+      </c>
+      <c r="N2">
         <v>16</v>
       </c>
-      <c r="K2">
-        <v>13559</v>
-      </c>
-      <c r="L2">
-        <v>257</v>
-      </c>
-      <c r="M2">
-        <v>205</v>
-      </c>
-      <c r="N2">
-        <v>10</v>
-      </c>
       <c r="O2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>1.72</v>
+        <v>1.76</v>
       </c>
       <c r="S2" s="2">
-        <v>0.1331</v>
+        <v>0.111</v>
       </c>
       <c r="T2">
-        <v>8.01</v>
+        <v>5.45</v>
       </c>
       <c r="U2">
-        <v>4.76</v>
+        <v>4.84</v>
       </c>
       <c r="V2">
         <v>2.2799999999999998</v>
       </c>
       <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>-1.6100000000000136</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42633.880312499998</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>10847</v>
+      </c>
+      <c r="F3">
+        <v>1310</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>32</v>
+      </c>
+      <c r="I3">
+        <v>100</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>7060</v>
+      </c>
+      <c r="L3">
+        <v>146</v>
+      </c>
+      <c r="M3">
+        <v>70</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1.76</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0.111</v>
+      </c>
+      <c r="T3">
+        <v>5.45</v>
+      </c>
+      <c r="U3">
+        <v>4.84</v>
+      </c>
+      <c r="V3">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I fixed an issue with the bollinger bands. They weren't calcualting properly
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +672,83 @@
       <c r="W3">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>-0.29999499999999557</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42635.817361111112</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>28</v>
+      </c>
+      <c r="E4">
+        <v>10331</v>
+      </c>
+      <c r="F4">
+        <v>1269</v>
+      </c>
+      <c r="G4">
+        <v>69</v>
+      </c>
+      <c r="H4">
+        <v>29</v>
+      </c>
+      <c r="I4">
+        <v>68</v>
+      </c>
+      <c r="J4">
+        <v>31</v>
+      </c>
+      <c r="K4">
+        <v>7075</v>
+      </c>
+      <c r="L4">
+        <v>145</v>
+      </c>
+      <c r="M4">
+        <v>61</v>
+      </c>
+      <c r="N4">
+        <v>26</v>
+      </c>
+      <c r="O4">
+        <v>12</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4">
+        <v>63.486785924529997</v>
+      </c>
+      <c r="R4">
+        <v>1.76</v>
+      </c>
+      <c r="S4" s="2">
+        <v>0.109</v>
+      </c>
+      <c r="T4" s="2">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="U4">
+        <v>4.84</v>
+      </c>
+      <c r="V4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Major code refactoring. The first phase of implementing a automatic repeater scanner and trader. Ran scans
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Bag</t>
+  </si>
+  <si>
+    <t>Down</t>
   </si>
 </sst>
 </file>
@@ -424,25 +427,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -592,6 +595,83 @@
       <c r="W2">
         <v>0</v>
       </c>
+      <c r="X2">
+        <v>-5.9997999999993112E-2</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>42648.663935185185</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <v>8602</v>
+      </c>
+      <c r="F3">
+        <v>1007</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>84</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="K3">
+        <v>6117</v>
+      </c>
+      <c r="L3">
+        <v>137</v>
+      </c>
+      <c r="M3">
+        <v>88</v>
+      </c>
+      <c r="N3">
+        <v>50</v>
+      </c>
+      <c r="O3">
+        <v>9</v>
+      </c>
+      <c r="P3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3">
+        <v>48.098617091043238</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>9.6699999999999994E-2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="U3">
+        <v>4.8</v>
+      </c>
+      <c r="V3">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Big changes. Added the repeater functions for a potential all night experiment. Ran trades
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/AAPL/AAPLBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -427,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +672,160 @@
       <c r="W3">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>-0.34999899999999684</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42649.612187500003</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>36</v>
+      </c>
+      <c r="E4">
+        <v>7436</v>
+      </c>
+      <c r="F4">
+        <v>787</v>
+      </c>
+      <c r="G4">
+        <v>63</v>
+      </c>
+      <c r="H4">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <v>86</v>
+      </c>
+      <c r="J4">
+        <v>13</v>
+      </c>
+      <c r="K4">
+        <v>5352</v>
+      </c>
+      <c r="L4">
+        <v>110</v>
+      </c>
+      <c r="M4">
+        <v>61</v>
+      </c>
+      <c r="N4">
+        <v>19</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4">
+        <v>35.483823948801813</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="T4" s="2">
+        <v>2.69E-2</v>
+      </c>
+      <c r="U4">
+        <v>4.82</v>
+      </c>
+      <c r="V4">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>-0.34999899999999684</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42649.635567129626</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>9051</v>
+      </c>
+      <c r="F5">
+        <v>1047</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
+      </c>
+      <c r="I5">
+        <v>90</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>6478</v>
+      </c>
+      <c r="L5">
+        <v>150</v>
+      </c>
+      <c r="M5">
+        <v>74</v>
+      </c>
+      <c r="N5">
+        <v>69</v>
+      </c>
+      <c r="O5">
+        <v>7</v>
+      </c>
+      <c r="P5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5">
+        <v>35.483823948801813</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2.69E-2</v>
+      </c>
+      <c r="U5">
+        <v>4.82</v>
+      </c>
+      <c r="V5">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>